<commit_message>
Adding day sfcWind in the xlsx CovidMIP with CMIP + additions #663.
</commit_message>
<xml_diff>
--- a/ece2cmor3/resources/miscellaneous-data-requests/cmip6-data-request-CovidMIP/cmvme_CMIP_ssp245_1_1-additional.xlsx
+++ b/ece2cmor3/resources/miscellaneous-data-requests/cmip6-data-request-CovidMIP/cmvme_CMIP_ssp245_1_1-additional.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="1" state="visible" r:id="rId2"/>
@@ -2234,7 +2234,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10810" uniqueCount="3220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10811" uniqueCount="3220">
   <si>
     <t xml:space="preserve">Notes on tables</t>
   </si>
@@ -34305,10 +34305,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AF30"/>
+  <dimension ref="A1:AF31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L31" activeCellId="0" sqref="L31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -36795,6 +36795,11 @@
       <c r="AD30" s="2"/>
       <c r="AE30" s="2"/>
       <c r="AF30" s="2"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L31" s="0" t="s">
+        <v>218</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -37603,11 +37608,14 @@
   </sheetPr>
   <dimension ref="A1:AF6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="L6" activeCellId="0" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.67"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="44.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>